<commit_message>
inpection tools improved, reconstruction parameters added, docs improved
</commit_message>
<xml_diff>
--- a/examples/KE123_indices.xlsx
+++ b/examples/KE123_indices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\projects\jyu\javelin\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060EA890-2B07-4198-B611-29BECEF544A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0253F4CC-943A-49E0-8D42-0E602C7A0B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="33">
   <si>
     <t>Throw</t>
   </si>
@@ -63,15 +63,6 @@
     <t>ForcePlatesRL</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -105,15 +96,6 @@
     <t>CameraLEDFrame</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -129,16 +111,31 @@
     <t>NumLeds</t>
   </si>
   <si>
-    <t>&lt;- Helmiina1_vt.mp4</t>
-  </si>
-  <si>
-    <t>&lt;- Helmiina2_oe.mp4</t>
-  </si>
-  <si>
-    <t>&lt;- Helmiina2_ot.mp4</t>
-  </si>
-  <si>
-    <t>&lt;- Helmiina2_ve.mp4</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>SyncDeltaRef</t>
+  </si>
+  <si>
+    <t>SyncDeltaLED</t>
+  </si>
+  <si>
+    <t>SyncDeltaFrame</t>
   </si>
 </sst>
 </file>
@@ -194,11 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C74B22-030D-4F29-AB8B-3607FB2E53EC}">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,57 +495,70 @@
     <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="15.109375" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>240</v>
@@ -556,10 +567,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F5" si="0">G2+IF(C2=240,IF(I2&gt;2,-1,0),IF(I2&gt;3,-1,0))</f>
+        <f>G2+IF(C2=240,IF(I2&gt;2,-1,0),IF(I2&gt;3,-1,0))</f>
         <v>0</v>
       </c>
       <c r="G2" s="3"/>
@@ -569,19 +580,30 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q2">
+        <f>H2-G2</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>((Q2+0.499)/C2+R2/1000)*C2</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>240</v>
@@ -590,32 +612,40 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3"/>
+        <f>ROUND(H3-S3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <f>I3-I2</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>((Q2+0.499)/C2+R3/1000)*C3</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>180</v>
@@ -624,32 +654,40 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3"/>
+        <f>ROUND(H4-S4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <f>I4-I2</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f>((Q2+0.499)/C2+R4/1000)*C4</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>180</v>
@@ -658,49 +696,40 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>1119</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1119</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1422</v>
-      </c>
-      <c r="I5" s="3">
-        <v>2</v>
-      </c>
+        <f>ROUND(H5-S5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1208</v>
-      </c>
-      <c r="M5" s="3">
-        <v>1262</v>
-      </c>
-      <c r="N5" s="3">
-        <v>1317</v>
-      </c>
-      <c r="O5" s="3">
-        <v>1350</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="R5">
+        <f>I5-I2</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>((Q2+0.499)/C2+R5/1000)*C5</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>240</v>
@@ -709,41 +738,43 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F25" si="1">G6+IF(C6=240,IF(I6&gt;2,-1,0),IF(I6&gt;3,-1,0))</f>
-        <v>1287</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1288</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1244</v>
-      </c>
-      <c r="I6" s="3">
-        <v>5</v>
-      </c>
+        <f t="shared" ref="F6:F25" si="0">ROUND(H6-S6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="Q6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q25" si="1">H6-G6</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6" si="2">((Q6+0.499)/C6+R6/1000)*C6</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>240</v>
@@ -752,41 +783,40 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>588</v>
-      </c>
-      <c r="G7" s="3">
-        <v>588</v>
-      </c>
-      <c r="H7" s="3">
-        <v>529</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="Q7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <f t="shared" ref="R7:R25" si="3">I7-I6</f>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7" si="4">((Q6+0.499)/C6+R7/1000)*C7</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>180</v>
@@ -795,41 +825,40 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>373</v>
-      </c>
-      <c r="G8" s="3">
-        <v>374</v>
-      </c>
-      <c r="H8" s="3">
-        <v>331</v>
-      </c>
-      <c r="I8" s="3">
-        <v>5</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="Q8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <f t="shared" ref="R8" si="5">I8-I6</f>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="S8" si="6">((Q6+0.499)/C6+R8/1000)*C8</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>180</v>
@@ -838,32 +867,40 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <f t="shared" ref="R9" si="7">I9-I6</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ref="S9" si="8">((Q6+0.499)/C6+R9/1000)*C9</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>240</v>
@@ -872,10 +909,10 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" s="3"/>
@@ -885,19 +922,30 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <f t="shared" ref="Q10:Q25" si="9">H10-G10</f>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ref="S10" si="10">((Q10+0.499)/C10+R10/1000)*C10</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>240</v>
@@ -906,32 +954,40 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <f t="shared" ref="R11:R25" si="11">I11-I10</f>
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ref="S11" si="12">((Q10+0.499)/C10+R11/1000)*C11</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1">
         <v>180</v>
@@ -940,32 +996,40 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <f t="shared" ref="R12" si="13">I12-I10</f>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ref="S12" si="14">((Q10+0.499)/C10+R12/1000)*C12</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
       </c>
       <c r="C13" s="1">
         <v>180</v>
@@ -974,32 +1038,40 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <f t="shared" ref="R13" si="15">I13-I10</f>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13" si="16">((Q10+0.499)/C10+R13/1000)*C13</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>240</v>
@@ -1008,10 +1080,10 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G14" s="3"/>
@@ -1021,19 +1093,30 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <f t="shared" ref="Q14:Q25" si="17">H14-G14</f>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ref="S14" si="18">((Q14+0.499)/C14+R14/1000)*C14</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>240</v>
@@ -1042,32 +1125,40 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <f t="shared" ref="R15:R25" si="19">I15-I14</f>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f t="shared" ref="S15" si="20">((Q14+0.499)/C14+R15/1000)*C15</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
         <v>180</v>
@@ -1076,32 +1167,40 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="4"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R16">
+        <f t="shared" ref="R16" si="21">I16-I14</f>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f t="shared" ref="S16" si="22">((Q14+0.499)/C14+R16/1000)*C16</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
         <v>180</v>
@@ -1110,32 +1209,40 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R17">
+        <f t="shared" ref="R17" si="23">I17-I14</f>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ref="S17" si="24">((Q14+0.499)/C14+R17/1000)*C17</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1">
         <v>240</v>
@@ -1144,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G18" s="3"/>
@@ -1157,19 +1264,30 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q18">
+        <f t="shared" ref="Q18:Q25" si="25">H18-G18</f>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" ref="S18" si="26">((Q18+0.499)/C18+R18/1000)*C18</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1">
         <v>240</v>
@@ -1178,32 +1296,40 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="4"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <f t="shared" ref="R19:R25" si="27">I19-I18</f>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" ref="S19" si="28">((Q18+0.499)/C18+R19/1000)*C19</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1">
         <v>180</v>
@@ -1212,32 +1338,40 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="4"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <f t="shared" ref="R20" si="29">I20-I18</f>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f t="shared" ref="S20" si="30">((Q18+0.499)/C18+R20/1000)*C20</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <v>180</v>
@@ -1246,32 +1380,40 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <f t="shared" ref="R21" si="31">I21-I18</f>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f t="shared" ref="S21" si="32">((Q18+0.499)/C18+R21/1000)*C21</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
         <v>240</v>
@@ -1280,10 +1422,10 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G22" s="3"/>
@@ -1293,19 +1435,30 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q22">
+        <f t="shared" ref="Q22:Q25" si="33">H22-G22</f>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f t="shared" ref="S22" si="34">((Q22+0.499)/C22+R22/1000)*C22</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1">
         <v>240</v>
@@ -1314,32 +1467,40 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="4"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <f t="shared" ref="R23:R25" si="35">I23-I22</f>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f t="shared" ref="S23" si="36">((Q22+0.499)/C22+R23/1000)*C23</f>
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1">
         <v>180</v>
@@ -1348,32 +1509,40 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="4"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <f t="shared" ref="R24" si="37">I24-I22</f>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ref="S24" si="38">((Q22+0.499)/C22+R24/1000)*C24</f>
+        <v>0.37424999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1">
         <v>180</v>
@@ -1382,33 +1551,38 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="4"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
+      <c r="R25">
+        <f t="shared" ref="R25" si="39">I25-I22</f>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f t="shared" ref="S25" si="40">((Q22+0.499)/C22+R25/1000)*C25</f>
+        <v>0.37424999999999997</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2 A3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update example _indices xlsx
</commit_message>
<xml_diff>
--- a/examples/KE123_indices.xlsx
+++ b/examples/KE123_indices.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\projects\jyu\javelin\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE4F675-CDAD-4901-B9B5-4D9EEBA25132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8B769D-3678-41DC-BB8F-0F99834D6635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sync" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C74B22-030D-4F29-AB8B-3607FB2E53EC}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +547,7 @@
         <v>240</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -592,7 +592,7 @@
         <v>240</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
@@ -633,7 +633,7 @@
         <v>180</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>16</v>
@@ -674,7 +674,7 @@
         <v>180</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
@@ -715,7 +715,7 @@
         <v>240</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -760,7 +760,7 @@
         <v>240</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -801,7 +801,7 @@
         <v>180</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -842,7 +842,7 @@
         <v>180</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
@@ -883,7 +883,7 @@
         <v>240</v>
       </c>
       <c r="D10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
@@ -928,7 +928,7 @@
         <v>240</v>
       </c>
       <c r="D11" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>16</v>
@@ -969,7 +969,7 @@
         <v>180</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
@@ -1010,7 +1010,7 @@
         <v>180</v>
       </c>
       <c r="D13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>16</v>
@@ -1051,7 +1051,7 @@
         <v>240</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>16</v>
@@ -1096,7 +1096,7 @@
         <v>240</v>
       </c>
       <c r="D15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1137,7 +1137,7 @@
         <v>180</v>
       </c>
       <c r="D16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1178,7 +1178,7 @@
         <v>180</v>
       </c>
       <c r="D17" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>16</v>
@@ -1219,7 +1219,7 @@
         <v>240</v>
       </c>
       <c r="D18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>16</v>
@@ -1264,7 +1264,7 @@
         <v>240</v>
       </c>
       <c r="D19" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
@@ -1305,7 +1305,7 @@
         <v>180</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1346,7 +1346,7 @@
         <v>180</v>
       </c>
       <c r="D21" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1387,7 +1387,7 @@
         <v>240</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
@@ -1432,7 +1432,7 @@
         <v>240</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>16</v>
@@ -1473,7 +1473,7 @@
         <v>180</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>16</v>
@@ -1514,7 +1514,7 @@
         <v>180</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>

</xml_diff>